<commit_message>
Some grammar and excess trimming
</commit_message>
<xml_diff>
--- a/deliverable0/Product_Backlog_RootDigital.xlsx
+++ b/deliverable0/Product_Backlog_RootDigital.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Repos\Root-Digital\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Repos\Root-Digital\deliverable0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F19390-CE9D-4734-916D-C962699D078A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5228B377-EF19-4B94-9890-8A458594021C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1935" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,8 +423,8 @@
   </sheetPr>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B24" sqref="B23:B24"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -695,9 +695,6 @@
       <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
       <c r="B22" s="5"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -705,9 +702,7 @@
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
+      <c r="A23" s="1"/>
       <c r="B23" s="5"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>

</xml_diff>